<commit_message>
plotting and raw data for the Lead circuit
</commit_message>
<xml_diff>
--- a/ControlLab/Lab3/Lag_rawData.xlsx
+++ b/ControlLab/Lab3/Lag_rawData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Control-Labs\ControlLab\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA624E0C-4E20-471C-90A1-015060CF5161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6367FCF-F9D0-4F30-939E-8644C637A010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3630" windowWidth="29040" windowHeight="15990" xr2:uid="{8664E146-489D-4B92-96D8-7C437F1D6661}"/>
+    <workbookView xWindow="-38520" yWindow="3930" windowWidth="38640" windowHeight="15990" xr2:uid="{8664E146-489D-4B92-96D8-7C437F1D6661}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B60639-DF05-4FE2-8011-A6C30A7ADAEF}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,7 +419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -432,8 +432,18 @@
       <c r="D2">
         <v>-9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <f>C2/B2</f>
+        <v>3.191919191919192</v>
+      </c>
+      <c r="J2">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -446,8 +456,18 @@
       <c r="D3">
         <v>-11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I14" si="0">C3/B3</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="J3">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
@@ -460,8 +480,18 @@
       <c r="D4">
         <v>-20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>2.9387755102040818</v>
+      </c>
+      <c r="J4">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23</v>
       </c>
@@ -474,8 +504,18 @@
       <c r="D5">
         <v>-32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2.6391752577319587</v>
+      </c>
+      <c r="J5">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>39</v>
       </c>
@@ -488,8 +528,18 @@
       <c r="D6">
         <v>-39</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>2.1224489795918369</v>
+      </c>
+      <c r="J6">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>65</v>
       </c>
@@ -502,8 +552,18 @@
       <c r="D7">
         <v>-51</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>65</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.510204081632653</v>
+      </c>
+      <c r="J7">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>108</v>
       </c>
@@ -516,8 +576,18 @@
       <c r="D8">
         <v>-50</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>108</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.0408163265306123</v>
+      </c>
+      <c r="J8">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>180</v>
       </c>
@@ -530,8 +600,18 @@
       <c r="D9">
         <v>-51</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>180</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.71717171717171713</v>
+      </c>
+      <c r="J9">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>300</v>
       </c>
@@ -544,8 +624,18 @@
       <c r="D10">
         <v>-39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>300</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.54545454545454553</v>
+      </c>
+      <c r="J10">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>500</v>
       </c>
@@ -558,8 +648,91 @@
       <c r="D11">
         <v>-25</v>
       </c>
+      <c r="H11">
+        <v>500</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.45918367346938777</v>
+      </c>
+      <c r="J11">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>800</v>
+      </c>
+      <c r="B12">
+        <v>1.98</v>
+      </c>
+      <c r="C12">
+        <v>0.84</v>
+      </c>
+      <c r="D12">
+        <v>-23</v>
+      </c>
+      <c r="H12">
+        <v>800</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.42424242424242425</v>
+      </c>
+      <c r="J12">
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>1.98</v>
+      </c>
+      <c r="C13">
+        <v>0.82</v>
+      </c>
+      <c r="D13">
+        <v>-14</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.41414141414141414</v>
+      </c>
+      <c r="J13">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1200</v>
+      </c>
+      <c r="B14">
+        <v>1.98</v>
+      </c>
+      <c r="C14">
+        <v>0.82</v>
+      </c>
+      <c r="D14">
+        <v>-10</v>
+      </c>
+      <c r="H14">
+        <v>1200</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.41414141414141414</v>
+      </c>
+      <c r="J14">
+        <v>-10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>